<commit_message>
Update version in schematics. Update all output files.
</commit_message>
<xml_diff>
--- a/Assembly/eva01/bom-eva01.xlsx
+++ b/Assembly/eva01/bom-eva01.xlsx
@@ -19,7 +19,7 @@
     <t>Bill of Materials</t>
   </si>
   <si>
-    <t>Date: Tuesday, 19 January 2016 10:26:56</t>
+    <t>Date: Tuesday, 09 February 2016 10:02:27</t>
   </si>
   <si>
     <t>Project: EVA01 Evaluation board for DevelBoard</t>
@@ -34,7 +34,7 @@
     <t>BOM files:</t>
   </si>
   <si>
-    <t>- tmp_bom-eva01.xls</t>
+    <t>- bom-eva01.xlsx</t>
   </si>
   <si>
     <t>NP=NON MONTARE!</t>
@@ -76,7 +76,7 @@
     <t>T.Qty</t>
   </si>
   <si>
-    <t>tmp_bom-eva01.xls</t>
+    <t>bom-eva01.xlsx</t>
   </si>
   <si>
     <t>Designator</t>

</xml_diff>

<commit_message>
Update and clean up.
</commit_message>
<xml_diff>
--- a/Assembly/eva01/bom-eva01.xlsx
+++ b/Assembly/eva01/bom-eva01.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -19,7 +19,7 @@
     <t>Bill of Materials</t>
   </si>
   <si>
-    <t>Date: Friday, 15 April 2016 16:29:05</t>
+    <t>Date: Friday, 17 June 2016 12:10:39</t>
   </si>
   <si>
     <t>Project: EVA01 Evaluation board for DevelBoard</t>
@@ -214,7 +214,7 @@
     <t>R1, R2, R3, R4, R5, R6, R7, R10, R63, R89, R90, R91, R92, R93, R94</t>
   </si>
   <si>
-    <t xml:space="preserve">NP  </t>
+    <t xml:space="preserve">NP    </t>
   </si>
   <si>
     <t>0603_[1608]</t>
@@ -226,13 +226,13 @@
     <t>R35</t>
   </si>
   <si>
-    <t xml:space="preserve">NP  (10k) </t>
+    <t xml:space="preserve">NP   (10k)  </t>
   </si>
   <si>
     <t>R36</t>
   </si>
   <si>
-    <t xml:space="preserve">NP  (1k) </t>
+    <t xml:space="preserve">NP   (1k)  </t>
   </si>
   <si>
     <t>R87</t>
@@ -292,7 +292,7 @@
     <t>C22</t>
   </si>
   <si>
-    <t xml:space="preserve">NP  (100nF) </t>
+    <t xml:space="preserve">NP   (100nF)  </t>
   </si>
   <si>
     <t>Ceramic X7R 50V</t>
@@ -445,7 +445,7 @@
     <t>L19</t>
   </si>
   <si>
-    <t xml:space="preserve">NP  (220 ohm @ 100MHz) </t>
+    <t xml:space="preserve">NP   (220 ohm @ 100MHz)  </t>
   </si>
   <si>
     <t>Ferrite Beat (WE 742792022)</t>
@@ -481,7 +481,7 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>NP  (IRLML6402)</t>
+    <t>NP   (IRLML6402)</t>
   </si>
   <si>
     <t>SOT-23</t>
@@ -723,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -732,6 +732,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,12 +743,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1043,121 +1040,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65" bestFit="1" customWidth="1"/>
-    <col min="7" max="29" width="10.7109375" customWidth="1"/>
-    <col min="30" max="95" width="138.7109375" customWidth="1"/>
+    <col min="3" max="95" width="50.7109375" customWidth="1"/>
+    <col min="4" max="95" width="50.7109375" customWidth="1"/>
+    <col min="5" max="95" width="50.7109375" customWidth="1"/>
+    <col min="6" max="95" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
@@ -1249,7 +1242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75">
+    <row r="26" spans="1:6">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1270,1277 +1263,1277 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="4">
-        <v>1</v>
-      </c>
-      <c r="B30" s="5">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="4">
-        <v>1</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="4">
+      <c r="A32" s="5">
         <v>3</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>3</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="4">
-        <v>1</v>
-      </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="4">
-        <v>1</v>
-      </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="4">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="4">
-        <v>1</v>
-      </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="A36" s="5">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="4">
-        <v>1</v>
-      </c>
-      <c r="B37" s="5">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="A37" s="5">
+        <v>1</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="4">
-        <v>1</v>
-      </c>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="4">
-        <v>1</v>
-      </c>
-      <c r="B39" s="5">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="A39" s="5">
+        <v>1</v>
+      </c>
+      <c r="B39" s="6">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="4">
-        <v>1</v>
-      </c>
-      <c r="B40" s="5">
-        <v>1</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="A40" s="5">
+        <v>1</v>
+      </c>
+      <c r="B40" s="6">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="4">
-        <v>1</v>
-      </c>
-      <c r="B41" s="5">
-        <v>1</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="A41" s="5">
+        <v>1</v>
+      </c>
+      <c r="B41" s="6">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="4">
-        <v>1</v>
-      </c>
-      <c r="B43" s="5">
-        <v>1</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="A43" s="5">
+        <v>1</v>
+      </c>
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="1:6" ht="90">
-      <c r="A45" s="4">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="5">
         <v>15</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="6">
         <v>15</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="4">
-        <v>1</v>
-      </c>
-      <c r="B46" s="5">
-        <v>1</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="A46" s="5">
+        <v>1</v>
+      </c>
+      <c r="B46" s="6">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="4">
-        <v>1</v>
-      </c>
-      <c r="B47" s="5">
-        <v>1</v>
-      </c>
-      <c r="C47" s="5" t="s">
+      <c r="A47" s="5">
+        <v>1</v>
+      </c>
+      <c r="B47" s="6">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="4">
-        <v>1</v>
-      </c>
-      <c r="B48" s="5">
-        <v>1</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="A48" s="5">
+        <v>1</v>
+      </c>
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="195">
-      <c r="A49" s="4">
+    <row r="49" spans="1:6">
+      <c r="A49" s="5">
         <v>26</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="6">
         <v>26</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="4">
-        <v>1</v>
-      </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="A50" s="5">
+        <v>1</v>
+      </c>
+      <c r="B50" s="6">
+        <v>1</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="4">
-        <v>1</v>
-      </c>
-      <c r="B51" s="5">
-        <v>1</v>
-      </c>
-      <c r="C51" s="5" t="s">
+      <c r="A51" s="5">
+        <v>1</v>
+      </c>
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="4">
+      <c r="A52" s="5">
         <v>3</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="6">
         <v>3</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="4">
+      <c r="A53" s="5">
         <v>2</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="6">
         <v>2</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="90">
-      <c r="A54" s="4">
+    <row r="54" spans="1:6">
+      <c r="A54" s="5">
         <v>13</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="6">
         <v>13</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="30">
-      <c r="A55" s="4">
+    <row r="55" spans="1:6">
+      <c r="A55" s="5">
         <v>5</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="6">
         <v>5</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="45">
-      <c r="A56" s="4">
+    <row r="56" spans="1:6">
+      <c r="A56" s="5">
         <v>6</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="6">
         <v>6</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="4">
-        <v>1</v>
-      </c>
-      <c r="B58" s="5">
-        <v>1</v>
-      </c>
-      <c r="C58" s="5" t="s">
+      <c r="A58" s="5">
+        <v>1</v>
+      </c>
+      <c r="B58" s="6">
+        <v>1</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="4">
+      <c r="A59" s="5">
         <v>2</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="6">
         <v>2</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="4">
+      <c r="A60" s="5">
         <v>2</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B60" s="6">
         <v>2</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="210">
-      <c r="A61" s="4">
+    <row r="61" spans="1:6">
+      <c r="A61" s="5">
         <v>30</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="6">
         <v>30</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="4">
+      <c r="A62" s="5">
         <v>3</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="6">
         <v>3</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="4">
-        <v>1</v>
-      </c>
-      <c r="B63" s="5">
-        <v>1</v>
-      </c>
-      <c r="C63" s="5" t="s">
+      <c r="A63" s="5">
+        <v>1</v>
+      </c>
+      <c r="B63" s="6">
+        <v>1</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="4">
-        <v>1</v>
-      </c>
-      <c r="B64" s="5">
-        <v>1</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="A64" s="5">
+        <v>1</v>
+      </c>
+      <c r="B64" s="6">
+        <v>1</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E64" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="60">
-      <c r="A65" s="4">
+    <row r="65" spans="1:6">
+      <c r="A65" s="5">
         <v>10</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="6">
         <v>10</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="6" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="4">
-        <v>1</v>
-      </c>
-      <c r="B66" s="5">
-        <v>1</v>
-      </c>
-      <c r="C66" s="5" t="s">
+      <c r="A66" s="5">
+        <v>1</v>
+      </c>
+      <c r="B66" s="6">
+        <v>1</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="4">
-        <v>1</v>
-      </c>
-      <c r="B67" s="5">
-        <v>1</v>
-      </c>
-      <c r="C67" s="5" t="s">
+      <c r="A67" s="5">
+        <v>1</v>
+      </c>
+      <c r="B67" s="6">
+        <v>1</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="4">
-        <v>1</v>
-      </c>
-      <c r="B69" s="5">
-        <v>1</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="A69" s="5">
+        <v>1</v>
+      </c>
+      <c r="B69" s="6">
+        <v>1</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30">
-      <c r="A70" s="4">
+    <row r="70" spans="1:6">
+      <c r="A70" s="5">
         <v>5</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="6">
         <v>5</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="6" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="4">
+      <c r="A71" s="5">
         <v>2</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="6">
         <v>2</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E71" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="6" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="4">
-        <v>1</v>
-      </c>
-      <c r="B72" s="5">
-        <v>1</v>
-      </c>
-      <c r="C72" s="5" t="s">
+      <c r="A72" s="5">
+        <v>1</v>
+      </c>
+      <c r="B72" s="6">
+        <v>1</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="4">
-        <v>1</v>
-      </c>
-      <c r="B74" s="5">
-        <v>1</v>
-      </c>
-      <c r="C74" s="5" t="s">
+      <c r="A74" s="5">
+        <v>1</v>
+      </c>
+      <c r="B74" s="6">
+        <v>1</v>
+      </c>
+      <c r="C74" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="4">
+      <c r="A76" s="5">
         <v>2</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="6">
         <v>2</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="6" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="4">
-        <v>1</v>
-      </c>
-      <c r="B77" s="5">
-        <v>1</v>
-      </c>
-      <c r="C77" s="5" t="s">
+      <c r="A77" s="5">
+        <v>1</v>
+      </c>
+      <c r="B77" s="6">
+        <v>1</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D77" s="6" t="s">
+      <c r="D77" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="4">
-        <v>1</v>
-      </c>
-      <c r="B78" s="5">
-        <v>1</v>
-      </c>
-      <c r="C78" s="5" t="s">
+      <c r="A78" s="5">
+        <v>1</v>
+      </c>
+      <c r="B78" s="6">
+        <v>1</v>
+      </c>
+      <c r="C78" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="4">
+      <c r="A79" s="5">
         <v>3</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="6">
         <v>3</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="60">
-      <c r="A80" s="4">
+    <row r="80" spans="1:6">
+      <c r="A80" s="5">
         <v>14</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="6">
         <v>14</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E80" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="6" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="4">
-        <v>1</v>
-      </c>
-      <c r="B82" s="5">
-        <v>1</v>
-      </c>
-      <c r="C82" s="5" t="s">
+      <c r="A82" s="5">
+        <v>1</v>
+      </c>
+      <c r="B82" s="6">
+        <v>1</v>
+      </c>
+      <c r="C82" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F82" s="6" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="4">
-        <v>1</v>
-      </c>
-      <c r="B84" s="5">
-        <v>1</v>
-      </c>
-      <c r="C84" s="5" t="s">
+      <c r="A84" s="5">
+        <v>1</v>
+      </c>
+      <c r="B84" s="6">
+        <v>1</v>
+      </c>
+      <c r="C84" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="6" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="4">
-        <v>1</v>
-      </c>
-      <c r="B85" s="5">
-        <v>1</v>
-      </c>
-      <c r="C85" s="5" t="s">
+      <c r="A85" s="5">
+        <v>1</v>
+      </c>
+      <c r="B85" s="6">
+        <v>1</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="F85" s="6" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="4">
-        <v>1</v>
-      </c>
-      <c r="B86" s="5">
-        <v>1</v>
-      </c>
-      <c r="C86" s="5" t="s">
+      <c r="A86" s="5">
+        <v>1</v>
+      </c>
+      <c r="B86" s="6">
+        <v>1</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E86" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F86" s="6" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="4">
-        <v>1</v>
-      </c>
-      <c r="B87" s="5">
-        <v>1</v>
-      </c>
-      <c r="C87" s="5" t="s">
+      <c r="A87" s="5">
+        <v>1</v>
+      </c>
+      <c r="B87" s="6">
+        <v>1</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F87" s="6" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="4">
-        <v>1</v>
-      </c>
-      <c r="B88" s="5">
-        <v>1</v>
-      </c>
-      <c r="C88" s="5" t="s">
+      <c r="A88" s="5">
+        <v>1</v>
+      </c>
+      <c r="B88" s="6">
+        <v>1</v>
+      </c>
+      <c r="C88" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F88" s="6" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="4">
-        <v>1</v>
-      </c>
-      <c r="B89" s="5">
-        <v>1</v>
-      </c>
-      <c r="C89" s="5" t="s">
+      <c r="A89" s="5">
+        <v>1</v>
+      </c>
+      <c r="B89" s="6">
+        <v>1</v>
+      </c>
+      <c r="C89" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="F89" s="6" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="4">
-        <v>1</v>
-      </c>
-      <c r="B90" s="5">
-        <v>1</v>
-      </c>
-      <c r="C90" s="5" t="s">
+      <c r="A90" s="5">
+        <v>1</v>
+      </c>
+      <c r="B90" s="6">
+        <v>1</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E90" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="F90" s="6" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="4">
-        <v>1</v>
-      </c>
-      <c r="B91" s="5">
-        <v>1</v>
-      </c>
-      <c r="C91" s="5" t="s">
+      <c r="A91" s="5">
+        <v>1</v>
+      </c>
+      <c r="B91" s="6">
+        <v>1</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E91" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F91" s="6" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="4">
+      <c r="A92" s="5">
         <v>2</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B92" s="6">
         <v>2</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E92" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F92" s="6" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="4">
-        <v>1</v>
-      </c>
-      <c r="B93" s="5">
-        <v>1</v>
-      </c>
-      <c r="C93" s="5" t="s">
+      <c r="A93" s="5">
+        <v>1</v>
+      </c>
+      <c r="B93" s="6">
+        <v>1</v>
+      </c>
+      <c r="C93" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E93" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F93" s="5" t="s">
+      <c r="F93" s="6" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="4">
-        <v>1</v>
-      </c>
-      <c r="B94" s="5">
-        <v>1</v>
-      </c>
-      <c r="C94" s="5" t="s">
+      <c r="A94" s="5">
+        <v>1</v>
+      </c>
+      <c r="B94" s="6">
+        <v>1</v>
+      </c>
+      <c r="C94" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F94" s="6" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="4">
-        <v>1</v>
-      </c>
-      <c r="B95" s="5">
-        <v>1</v>
-      </c>
-      <c r="C95" s="5" t="s">
+      <c r="A95" s="5">
+        <v>1</v>
+      </c>
+      <c r="B95" s="6">
+        <v>1</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E95" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F95" s="6" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A57:F57"/>
     <mergeCell ref="A68:F68"/>
     <mergeCell ref="A73:F73"/>
     <mergeCell ref="A75:F75"/>
     <mergeCell ref="A81:F81"/>
     <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>